<commit_message>
Added copy of sandbox ffm
</commit_message>
<xml_diff>
--- a/pivoted_statements.xlsx
+++ b/pivoted_statements.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/03a4090e471ff419/Documents/GitHub/finevalgroup/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_23F921EDF7AB0F259F2D4CF0FD03274148D49E97" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F39D66C-309F-44B1-AB57-410966EEFFD4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -265,8 +259,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,21 +323,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -381,7 +367,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -415,7 +401,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -450,10 +435,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -626,22 +610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -667,7 +643,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -693,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -719,7 +695,7 @@
         <v>1602.67</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -745,7 +721,7 @@
         <v>5281.52</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -771,7 +747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -797,7 +773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -823,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -849,7 +825,7 @@
         <v>370.94</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -875,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -901,7 +877,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
@@ -927,7 +903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -953,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -979,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1005,7 +981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1031,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -1057,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
@@ -1083,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1109,7 +1085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1135,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1161,7 +1137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -1187,7 +1163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
         <v>28</v>
       </c>
@@ -1213,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
@@ -1239,7 +1215,7 @@
         <v>596.25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1265,7 +1241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1291,7 +1267,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1317,7 +1293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
@@ -1328,10 +1304,10 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>158.08000000000001</v>
+        <v>158.08</v>
       </c>
       <c r="E27">
-        <v>158.08000000000001</v>
+        <v>158.08</v>
       </c>
       <c r="F27">
         <v>1003.73</v>
@@ -1343,7 +1319,7 @@
         <v>157.72</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -1369,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1395,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
         <v>36</v>
       </c>
@@ -1421,7 +1397,7 @@
         <v>1642.46</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
@@ -1447,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -1499,7 +1475,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -1516,7 +1492,7 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>18.079999999999998</v>
+        <v>18.08</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -1525,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -1551,7 +1527,7 @@
         <v>-9337.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1577,7 +1553,7 @@
         <v>13495</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
         <v>43</v>
       </c>
@@ -1603,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1614,7 +1590,7 @@
         <v>131.25</v>
       </c>
       <c r="D38">
-        <v>158.08000000000001</v>
+        <v>158.08</v>
       </c>
       <c r="E38">
         <v>239.09</v>
@@ -1629,7 +1605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
         <v>45</v>
       </c>
@@ -1655,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
@@ -1681,7 +1657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
         <v>47</v>
       </c>
@@ -1707,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
         <v>48</v>
       </c>
@@ -1733,7 +1709,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
@@ -1759,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
@@ -1785,7 +1761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
@@ -1811,7 +1787,7 @@
         <v>23436.29</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
@@ -1837,7 +1813,7 @@
         <v>23436.29</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
         <v>53</v>
       </c>
@@ -1863,7 +1839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -1889,7 +1865,7 @@
         <v>1602.67</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
         <v>55</v>
       </c>
@@ -1915,7 +1891,7 @@
         <v>5281.52</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
         <v>56</v>
       </c>
@@ -1941,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
         <v>57</v>
       </c>
@@ -1967,7 +1943,7 @@
         <v>2001</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
         <v>58</v>
       </c>
@@ -1993,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
         <v>59</v>
       </c>
@@ -2004,10 +1980,10 @@
         <v>0</v>
       </c>
       <c r="D53">
-        <v>158.08000000000001</v>
+        <v>158.08</v>
       </c>
       <c r="E53">
-        <v>158.08000000000001</v>
+        <v>158.08</v>
       </c>
       <c r="F53">
         <v>1003.73</v>
@@ -2019,7 +1995,7 @@
         <v>157.72</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
         <v>60</v>
       </c>
@@ -2039,13 +2015,13 @@
         <v>10841.29</v>
       </c>
       <c r="G54">
-        <v>9941.2900000000009</v>
+        <v>9941.290000000001</v>
       </c>
       <c r="H54">
-        <v>9941.2900000000009</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9941.290000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
         <v>61</v>
       </c>
@@ -2071,7 +2047,7 @@
         <v>6131.33</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
         <v>62</v>
       </c>
@@ -2097,7 +2073,7 @@
         <v>-7695.04</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
         <v>63</v>
       </c>
@@ -2123,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
         <v>64</v>
       </c>
@@ -2149,7 +2125,7 @@
         <v>13495</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
@@ -2175,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
         <v>66</v>
       </c>
@@ -2186,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="D60">
-        <v>158.08000000000001</v>
+        <v>158.08</v>
       </c>
       <c r="E60">
         <v>197.18</v>
@@ -2201,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
         <v>67</v>
       </c>
@@ -2212,7 +2188,7 @@
         <v>131.25</v>
       </c>
       <c r="D61">
-        <v>589.08000000000004</v>
+        <v>589.08</v>
       </c>
       <c r="E61">
         <v>936.09</v>
@@ -2227,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
         <v>68</v>
       </c>
@@ -2253,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
         <v>69</v>
       </c>
@@ -2279,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
         <v>70</v>
       </c>
@@ -2305,7 +2281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
         <v>71</v>
       </c>
@@ -2331,7 +2307,7 @@
         <v>31131.33</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
         <v>72</v>
       </c>
@@ -2357,7 +2333,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
         <v>73</v>
       </c>
@@ -2383,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
         <v>74</v>
       </c>
@@ -2409,7 +2385,7 @@
         <v>2658.77</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
         <v>75</v>
       </c>
@@ -2426,16 +2402,16 @@
         <v>46.4</v>
       </c>
       <c r="F69">
-        <v>4370.9399999999996</v>
+        <v>4370.94</v>
       </c>
       <c r="G69">
-        <v>4370.9399999999996</v>
+        <v>4370.94</v>
       </c>
       <c r="H69">
-        <v>4370.9399999999996</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+        <v>4370.94</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
         <v>76</v>
       </c>
@@ -2461,7 +2437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
         <v>77</v>
       </c>
@@ -2487,7 +2463,7 @@
         <v>13495</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
         <v>78</v>
       </c>
@@ -2513,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
         <v>79</v>
       </c>

</xml_diff>